<commit_message>
Added Encoders interrupts in both encoders and updated PinMap + VBA script on the PinMap file
</commit_message>
<xml_diff>
--- a/RobotProject_PinMap.xlsx
+++ b/RobotProject_PinMap.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaizi\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaizi\Desktop\Robot_Project_IFX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="136">
   <si>
     <t>X102</t>
   </si>
@@ -405,6 +405,33 @@
   </si>
   <si>
     <t>Encoder Inputs</t>
+  </si>
+  <si>
+    <t>En A H-Bridge</t>
+  </si>
+  <si>
+    <t>EN B H-Bridge</t>
+  </si>
+  <si>
+    <t>IN4 H-Bridge</t>
+  </si>
+  <si>
+    <t>IN 2 H-Bridge</t>
+  </si>
+  <si>
+    <t>Input Encoder 2</t>
+  </si>
+  <si>
+    <t>Input Encoder 1</t>
+  </si>
+  <si>
+    <t>PWM 1 -&gt; IN 1 H bridge</t>
+  </si>
+  <si>
+    <t>PWM 2 -&gt; IN 3 H bridge</t>
+  </si>
+  <si>
+    <t>blabla</t>
   </si>
 </sst>
 </file>
@@ -525,7 +552,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -831,32 +858,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -978,7 +979,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -1059,58 +1060,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="2" builtinId="20"/>
@@ -1393,14 +1384,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="20.140625" bestFit="1" customWidth="1"/>
@@ -1441,12 +1438,12 @@
       <c r="T2" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="U2" s="55" t="s">
+      <c r="U2" s="45" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="40" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2"/>
@@ -1488,7 +1485,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="41" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2"/>
@@ -1505,7 +1502,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="51" t="s">
+      <c r="H4" s="41" t="s">
         <v>4</v>
       </c>
       <c r="K4" s="1"/>
@@ -1682,6 +1679,9 @@
       <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="J9" s="28" t="s">
+        <v>132</v>
+      </c>
       <c r="K9" s="1" t="s">
         <v>50</v>
       </c>
@@ -1852,6 +1852,9 @@
       <c r="P13" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="Q13" s="28" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="14" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
@@ -1872,6 +1875,9 @@
       <c r="G14" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="J14" s="28" t="s">
+        <v>130</v>
+      </c>
       <c r="K14" s="1" t="s">
         <v>60</v>
       </c>
@@ -1889,6 +1895,9 @@
       </c>
       <c r="P14" s="1" t="s">
         <v>61</v>
+      </c>
+      <c r="Q14" s="28" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1910,6 +1919,9 @@
       <c r="G15" s="17" t="s">
         <v>26</v>
       </c>
+      <c r="J15" s="28" t="s">
+        <v>129</v>
+      </c>
       <c r="K15" s="1" t="s">
         <v>62</v>
       </c>
@@ -1927,6 +1939,9 @@
       </c>
       <c r="P15" s="1" t="s">
         <v>63</v>
+      </c>
+      <c r="Q15" s="28" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1948,6 +1963,9 @@
       <c r="G16" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="H16" s="28" t="s">
+        <v>134</v>
+      </c>
       <c r="K16" s="1" t="s">
         <v>64</v>
       </c>
@@ -2023,6 +2041,9 @@
       </c>
       <c r="G18" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>133</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>68</v>
@@ -2251,866 +2272,884 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="44"/>
-      <c r="L30" s="44"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="44"/>
-      <c r="O30" s="34"/>
-      <c r="P30" s="34"/>
-      <c r="Q30" s="35"/>
+      <c r="B30" s="49" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="D30" s="50" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="46"/>
+      <c r="P30" s="46"/>
+      <c r="Q30" s="46"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="37"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="38"/>
-      <c r="M31" s="38"/>
-      <c r="N31" s="38"/>
-      <c r="O31" s="38"/>
-      <c r="P31" s="38"/>
-      <c r="Q31" s="39"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="46"/>
+    </row>
+    <row r="32" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="38"/>
-      <c r="L32" s="38"/>
-      <c r="M32" s="38"/>
-      <c r="N32" s="38"/>
-      <c r="O32" s="38"/>
-      <c r="P32" s="38"/>
-      <c r="Q32" s="39"/>
+      <c r="B32" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="46"/>
+      <c r="P32" s="46"/>
+      <c r="Q32" s="46"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="38"/>
-      <c r="N33" s="38"/>
-      <c r="O33" s="38"/>
-      <c r="P33" s="38"/>
-      <c r="Q33" s="39"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="46"/>
+      <c r="P33" s="46"/>
+      <c r="Q33" s="46"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="37"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="38"/>
-      <c r="J34" s="38"/>
-      <c r="K34" s="38"/>
-      <c r="L34" s="38"/>
-      <c r="M34" s="38"/>
-      <c r="N34" s="38"/>
-      <c r="O34" s="38"/>
-      <c r="P34" s="38"/>
-      <c r="Q34" s="39"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="46"/>
+      <c r="M34" s="46"/>
+      <c r="N34" s="46"/>
+      <c r="O34" s="46"/>
+      <c r="P34" s="46"/>
+      <c r="Q34" s="46"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="36" t="s">
+      <c r="A35" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="37"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="38"/>
-      <c r="M35" s="38"/>
-      <c r="N35" s="38"/>
-      <c r="O35" s="38"/>
-      <c r="P35" s="38"/>
-      <c r="Q35" s="39"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="46"/>
+      <c r="N35" s="46"/>
+      <c r="O35" s="46"/>
+      <c r="P35" s="46"/>
+      <c r="Q35" s="46"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="37"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38"/>
-      <c r="I36" s="38"/>
-      <c r="J36" s="38"/>
-      <c r="K36" s="38"/>
-      <c r="L36" s="38"/>
-      <c r="M36" s="38"/>
-      <c r="N36" s="38"/>
-      <c r="O36" s="38"/>
-      <c r="P36" s="38"/>
-      <c r="Q36" s="39"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="46"/>
+      <c r="N36" s="46"/>
+      <c r="O36" s="46"/>
+      <c r="P36" s="46"/>
+      <c r="Q36" s="46"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
+      <c r="A37" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="37"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
-      <c r="J37" s="38"/>
-      <c r="K37" s="38"/>
-      <c r="L37" s="38"/>
-      <c r="M37" s="38"/>
-      <c r="N37" s="38"/>
-      <c r="O37" s="38"/>
-      <c r="P37" s="38"/>
-      <c r="Q37" s="39"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="46"/>
+      <c r="N37" s="46"/>
+      <c r="O37" s="46"/>
+      <c r="P37" s="46"/>
+      <c r="Q37" s="46"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="37"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="38"/>
-      <c r="L38" s="38"/>
-      <c r="M38" s="38"/>
-      <c r="N38" s="38"/>
-      <c r="O38" s="38"/>
-      <c r="P38" s="38"/>
-      <c r="Q38" s="39"/>
+      <c r="B38" s="46"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
+      <c r="N38" s="46"/>
+      <c r="O38" s="46"/>
+      <c r="P38" s="46"/>
+      <c r="Q38" s="46"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="38"/>
-      <c r="I39" s="38"/>
-      <c r="J39" s="38"/>
-      <c r="K39" s="38"/>
-      <c r="L39" s="38"/>
-      <c r="M39" s="38"/>
-      <c r="N39" s="38"/>
-      <c r="O39" s="38"/>
-      <c r="P39" s="38"/>
-      <c r="Q39" s="39"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="46"/>
+      <c r="N39" s="46"/>
+      <c r="O39" s="46"/>
+      <c r="P39" s="46"/>
+      <c r="Q39" s="46"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="36" t="s">
+      <c r="A40" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="B40" s="37"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="38"/>
-      <c r="K40" s="38"/>
-      <c r="L40" s="38"/>
-      <c r="M40" s="38"/>
-      <c r="N40" s="38"/>
-      <c r="O40" s="38"/>
-      <c r="P40" s="38"/>
-      <c r="Q40" s="39"/>
+      <c r="B40" s="46"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="50"/>
+      <c r="I40" s="50"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="46"/>
+      <c r="N40" s="46"/>
+      <c r="O40" s="46"/>
+      <c r="P40" s="46"/>
+      <c r="Q40" s="46"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B41" s="37"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="38"/>
-      <c r="J41" s="38"/>
-      <c r="K41" s="38"/>
-      <c r="L41" s="38"/>
-      <c r="M41" s="38"/>
-      <c r="N41" s="38"/>
-      <c r="O41" s="38"/>
-      <c r="P41" s="38"/>
-      <c r="Q41" s="39"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="46"/>
+      <c r="M41" s="46"/>
+      <c r="N41" s="46"/>
+      <c r="O41" s="46"/>
+      <c r="P41" s="46"/>
+      <c r="Q41" s="46"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="37"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="38"/>
-      <c r="J42" s="38"/>
-      <c r="K42" s="38"/>
-      <c r="L42" s="38"/>
-      <c r="M42" s="38"/>
-      <c r="N42" s="38"/>
-      <c r="O42" s="38"/>
-      <c r="P42" s="38"/>
-      <c r="Q42" s="39"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="46"/>
+      <c r="M42" s="46"/>
+      <c r="N42" s="46"/>
+      <c r="O42" s="46"/>
+      <c r="P42" s="46"/>
+      <c r="Q42" s="46"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="36" t="s">
+      <c r="A43" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="37"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
-      <c r="J43" s="38"/>
-      <c r="K43" s="38"/>
-      <c r="L43" s="38"/>
-      <c r="M43" s="38"/>
-      <c r="N43" s="38"/>
-      <c r="O43" s="38"/>
-      <c r="P43" s="38"/>
-      <c r="Q43" s="39"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="46"/>
+      <c r="M43" s="46"/>
+      <c r="N43" s="46"/>
+      <c r="O43" s="46"/>
+      <c r="P43" s="46"/>
+      <c r="Q43" s="46"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="36" t="s">
+      <c r="A44" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="37"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="38"/>
-      <c r="L44" s="38"/>
-      <c r="M44" s="38"/>
-      <c r="N44" s="38"/>
-      <c r="O44" s="38"/>
-      <c r="P44" s="38"/>
-      <c r="Q44" s="39"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="46"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="46"/>
+      <c r="L44" s="46"/>
+      <c r="M44" s="46"/>
+      <c r="N44" s="46"/>
+      <c r="O44" s="46"/>
+      <c r="P44" s="46"/>
+      <c r="Q44" s="46"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="34" t="s">
         <v>96</v>
       </c>
       <c r="B45" s="47"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="38"/>
-      <c r="K45" s="38"/>
-      <c r="L45" s="38"/>
-      <c r="M45" s="38"/>
-      <c r="N45" s="38"/>
-      <c r="O45" s="38"/>
-      <c r="P45" s="38"/>
-      <c r="Q45" s="39"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="46"/>
+      <c r="K45" s="46"/>
+      <c r="L45" s="46"/>
+      <c r="M45" s="46"/>
+      <c r="N45" s="46"/>
+      <c r="O45" s="46"/>
+      <c r="P45" s="46"/>
+      <c r="Q45" s="46"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="36" t="s">
+      <c r="A46" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="37"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
-      <c r="K46" s="38"/>
-      <c r="L46" s="38"/>
-      <c r="M46" s="38"/>
-      <c r="N46" s="38"/>
-      <c r="O46" s="38"/>
-      <c r="P46" s="38"/>
-      <c r="Q46" s="39"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="46"/>
+      <c r="M46" s="46"/>
+      <c r="N46" s="46"/>
+      <c r="O46" s="46"/>
+      <c r="P46" s="46"/>
+      <c r="Q46" s="46"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="37"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="38"/>
-      <c r="J47" s="38"/>
-      <c r="K47" s="38"/>
-      <c r="L47" s="38"/>
-      <c r="M47" s="38"/>
-      <c r="N47" s="38"/>
-      <c r="O47" s="38"/>
-      <c r="P47" s="38"/>
-      <c r="Q47" s="39"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
+      <c r="M47" s="46"/>
+      <c r="N47" s="46"/>
+      <c r="O47" s="46"/>
+      <c r="P47" s="46"/>
+      <c r="Q47" s="46"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="36" t="s">
+      <c r="A48" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="B48" s="37"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38"/>
-      <c r="J48" s="38"/>
-      <c r="K48" s="38"/>
-      <c r="L48" s="38"/>
-      <c r="M48" s="38"/>
-      <c r="N48" s="38"/>
-      <c r="O48" s="38"/>
-      <c r="P48" s="38"/>
-      <c r="Q48" s="39"/>
+      <c r="B48" s="46"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="46"/>
+      <c r="J48" s="46"/>
+      <c r="K48" s="46"/>
+      <c r="L48" s="46"/>
+      <c r="M48" s="46"/>
+      <c r="N48" s="46"/>
+      <c r="O48" s="46"/>
+      <c r="P48" s="46"/>
+      <c r="Q48" s="46"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A49" s="36" t="s">
+      <c r="A49" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="37"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="38"/>
-      <c r="J49" s="38"/>
-      <c r="K49" s="38"/>
-      <c r="L49" s="38"/>
-      <c r="M49" s="38"/>
-      <c r="N49" s="38"/>
-      <c r="O49" s="38"/>
-      <c r="P49" s="38"/>
-      <c r="Q49" s="39"/>
+      <c r="B49" s="46"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="46"/>
+      <c r="G49" s="46"/>
+      <c r="H49" s="46"/>
+      <c r="I49" s="46"/>
+      <c r="J49" s="46"/>
+      <c r="K49" s="46"/>
+      <c r="L49" s="46"/>
+      <c r="M49" s="46"/>
+      <c r="N49" s="46"/>
+      <c r="O49" s="46"/>
+      <c r="P49" s="46"/>
+      <c r="Q49" s="46"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A50" s="48" t="s">
+      <c r="A50" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="49"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
-      <c r="I50" s="38"/>
-      <c r="J50" s="38"/>
-      <c r="K50" s="44"/>
-      <c r="L50" s="44"/>
-      <c r="M50" s="38"/>
-      <c r="N50" s="38"/>
-      <c r="O50" s="38"/>
-      <c r="P50" s="38"/>
-      <c r="Q50" s="39"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="50"/>
+      <c r="L50" s="50"/>
+      <c r="M50" s="46"/>
+      <c r="N50" s="46"/>
+      <c r="O50" s="46"/>
+      <c r="P50" s="46"/>
+      <c r="Q50" s="46"/>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A51" s="36" t="s">
+      <c r="A51" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="B51" s="37"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="38"/>
-      <c r="H51" s="38"/>
-      <c r="I51" s="38"/>
-      <c r="J51" s="40"/>
-      <c r="K51" s="40"/>
-      <c r="L51" s="40"/>
-      <c r="M51" s="40"/>
-      <c r="N51" s="40"/>
-      <c r="O51" s="40"/>
-      <c r="P51" s="40"/>
-      <c r="Q51" s="41"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52" s="36" t="s">
+      <c r="B51" s="46"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="46"/>
+      <c r="J51" s="48"/>
+      <c r="K51" s="48"/>
+      <c r="L51" s="48"/>
+      <c r="M51" s="48"/>
+      <c r="N51" s="48"/>
+      <c r="O51" s="48"/>
+      <c r="P51" s="48"/>
+      <c r="Q51" s="48"/>
+    </row>
+    <row r="52" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="44"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="38"/>
-      <c r="H52" s="38"/>
-      <c r="I52" s="38"/>
-      <c r="J52" s="38"/>
-      <c r="K52" s="38"/>
-      <c r="L52" s="38"/>
-      <c r="M52" s="38"/>
-      <c r="N52" s="40"/>
-      <c r="O52" s="40"/>
-      <c r="P52" s="40"/>
-      <c r="Q52" s="41"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="46"/>
+      <c r="G52" s="46"/>
+      <c r="H52" s="46"/>
+      <c r="I52" s="46"/>
+      <c r="J52" s="46"/>
+      <c r="K52" s="46"/>
+      <c r="L52" s="46"/>
+      <c r="M52" s="46"/>
+      <c r="N52" s="48"/>
+      <c r="O52" s="48"/>
+      <c r="P52" s="48"/>
+      <c r="Q52" s="48"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53" s="36" t="s">
+      <c r="A53" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="44"/>
-      <c r="C53" s="44"/>
-      <c r="D53" s="44"/>
-      <c r="E53" s="44"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="38"/>
-      <c r="J53" s="38"/>
-      <c r="K53" s="40"/>
-      <c r="L53" s="40"/>
-      <c r="M53" s="40"/>
-      <c r="N53" s="40"/>
-      <c r="O53" s="40"/>
-      <c r="P53" s="40"/>
-      <c r="Q53" s="41"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="46"/>
+      <c r="J53" s="46"/>
+      <c r="K53" s="48"/>
+      <c r="L53" s="48"/>
+      <c r="M53" s="48"/>
+      <c r="N53" s="48"/>
+      <c r="O53" s="48"/>
+      <c r="P53" s="48"/>
+      <c r="Q53" s="48"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A54" s="36" t="s">
+      <c r="A54" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="B54" s="42"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="40"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="38"/>
-      <c r="J54" s="38"/>
-      <c r="K54" s="40"/>
-      <c r="L54" s="40"/>
-      <c r="M54" s="40"/>
-      <c r="N54" s="40"/>
-      <c r="O54" s="40"/>
-      <c r="P54" s="40"/>
-      <c r="Q54" s="41"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="48"/>
+      <c r="E54" s="48"/>
+      <c r="F54" s="48"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="48"/>
+      <c r="L54" s="48"/>
+      <c r="M54" s="48"/>
+      <c r="N54" s="48"/>
+      <c r="O54" s="48"/>
+      <c r="P54" s="48"/>
+      <c r="Q54" s="48"/>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A55" s="36" t="s">
+      <c r="A55" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="42"/>
-      <c r="C55" s="40"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="40"/>
-      <c r="K55" s="40"/>
-      <c r="L55" s="40"/>
-      <c r="M55" s="40"/>
-      <c r="N55" s="40"/>
-      <c r="O55" s="40"/>
-      <c r="P55" s="40"/>
-      <c r="Q55" s="41"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="48"/>
+      <c r="F55" s="48"/>
+      <c r="G55" s="48"/>
+      <c r="H55" s="48"/>
+      <c r="I55" s="48"/>
+      <c r="J55" s="48"/>
+      <c r="K55" s="48"/>
+      <c r="L55" s="48"/>
+      <c r="M55" s="48"/>
+      <c r="N55" s="48"/>
+      <c r="O55" s="48"/>
+      <c r="P55" s="48"/>
+      <c r="Q55" s="48"/>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A56" s="36" t="s">
+      <c r="A56" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="B56" s="42"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="40"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="40"/>
-      <c r="J56" s="40"/>
-      <c r="K56" s="40"/>
-      <c r="L56" s="40"/>
-      <c r="M56" s="40"/>
-      <c r="N56" s="40"/>
-      <c r="O56" s="40"/>
-      <c r="P56" s="40"/>
-      <c r="Q56" s="41"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="48"/>
+      <c r="E56" s="48"/>
+      <c r="F56" s="48"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="48"/>
+      <c r="I56" s="48"/>
+      <c r="J56" s="48"/>
+      <c r="K56" s="48"/>
+      <c r="L56" s="48"/>
+      <c r="M56" s="48"/>
+      <c r="N56" s="48"/>
+      <c r="O56" s="48"/>
+      <c r="P56" s="48"/>
+      <c r="Q56" s="48"/>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A57" s="36" t="s">
+      <c r="A57" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="B57" s="42"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="40"/>
-      <c r="E57" s="40"/>
-      <c r="F57" s="40"/>
-      <c r="G57" s="40"/>
-      <c r="H57" s="40"/>
-      <c r="I57" s="40"/>
-      <c r="J57" s="40"/>
-      <c r="K57" s="40"/>
-      <c r="L57" s="40"/>
-      <c r="M57" s="40"/>
-      <c r="N57" s="40"/>
-      <c r="O57" s="40"/>
-      <c r="P57" s="40"/>
-      <c r="Q57" s="41"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="48"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="48"/>
+      <c r="K57" s="48"/>
+      <c r="L57" s="48"/>
+      <c r="M57" s="48"/>
+      <c r="N57" s="48"/>
+      <c r="O57" s="48"/>
+      <c r="P57" s="48"/>
+      <c r="Q57" s="48"/>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A58" s="36" t="s">
+      <c r="A58" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="42"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="40"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="40"/>
-      <c r="I58" s="40"/>
-      <c r="J58" s="40"/>
-      <c r="K58" s="40"/>
-      <c r="L58" s="40"/>
-      <c r="M58" s="40"/>
-      <c r="N58" s="40"/>
-      <c r="O58" s="40"/>
-      <c r="P58" s="40"/>
-      <c r="Q58" s="41"/>
+      <c r="B58" s="48"/>
+      <c r="C58" s="48"/>
+      <c r="D58" s="48"/>
+      <c r="E58" s="48"/>
+      <c r="F58" s="48"/>
+      <c r="G58" s="48"/>
+      <c r="H58" s="48"/>
+      <c r="I58" s="48"/>
+      <c r="J58" s="48"/>
+      <c r="K58" s="48"/>
+      <c r="L58" s="48"/>
+      <c r="M58" s="48"/>
+      <c r="N58" s="48"/>
+      <c r="O58" s="48"/>
+      <c r="P58" s="48"/>
+      <c r="Q58" s="48"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A59" s="36" t="s">
+      <c r="A59" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="B59" s="42"/>
-      <c r="C59" s="40"/>
-      <c r="D59" s="40"/>
-      <c r="E59" s="40"/>
-      <c r="F59" s="40"/>
-      <c r="G59" s="40"/>
-      <c r="H59" s="40"/>
-      <c r="I59" s="40"/>
-      <c r="J59" s="40"/>
-      <c r="K59" s="40"/>
-      <c r="L59" s="40"/>
-      <c r="M59" s="40"/>
-      <c r="N59" s="40"/>
-      <c r="O59" s="40"/>
-      <c r="P59" s="40"/>
-      <c r="Q59" s="41"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="48"/>
+      <c r="E59" s="48"/>
+      <c r="F59" s="48"/>
+      <c r="G59" s="48"/>
+      <c r="H59" s="48"/>
+      <c r="I59" s="48"/>
+      <c r="J59" s="48"/>
+      <c r="K59" s="48"/>
+      <c r="L59" s="48"/>
+      <c r="M59" s="48"/>
+      <c r="N59" s="48"/>
+      <c r="O59" s="48"/>
+      <c r="P59" s="48"/>
+      <c r="Q59" s="48"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A60" s="36" t="s">
+      <c r="A60" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="B60" s="42"/>
-      <c r="C60" s="40"/>
-      <c r="D60" s="40"/>
-      <c r="E60" s="40"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="40"/>
-      <c r="H60" s="40"/>
-      <c r="I60" s="40"/>
-      <c r="J60" s="40"/>
-      <c r="K60" s="40"/>
-      <c r="L60" s="40"/>
-      <c r="M60" s="40"/>
-      <c r="N60" s="40"/>
-      <c r="O60" s="40"/>
-      <c r="P60" s="40"/>
-      <c r="Q60" s="41"/>
+      <c r="B60" s="48"/>
+      <c r="C60" s="48"/>
+      <c r="D60" s="48"/>
+      <c r="E60" s="48"/>
+      <c r="F60" s="48"/>
+      <c r="G60" s="48"/>
+      <c r="H60" s="48"/>
+      <c r="I60" s="48"/>
+      <c r="J60" s="48"/>
+      <c r="K60" s="48"/>
+      <c r="L60" s="48"/>
+      <c r="M60" s="48"/>
+      <c r="N60" s="48"/>
+      <c r="O60" s="48"/>
+      <c r="P60" s="48"/>
+      <c r="Q60" s="48"/>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A61" s="36" t="s">
+      <c r="A61" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="B61" s="42"/>
-      <c r="C61" s="40"/>
-      <c r="D61" s="40"/>
-      <c r="E61" s="40"/>
-      <c r="F61" s="40"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="40"/>
-      <c r="I61" s="40"/>
-      <c r="J61" s="40"/>
-      <c r="K61" s="40"/>
-      <c r="L61" s="40"/>
-      <c r="M61" s="40"/>
-      <c r="N61" s="40"/>
-      <c r="O61" s="40"/>
-      <c r="P61" s="40"/>
-      <c r="Q61" s="41"/>
+      <c r="B61" s="48"/>
+      <c r="C61" s="48"/>
+      <c r="D61" s="48"/>
+      <c r="E61" s="48"/>
+      <c r="F61" s="48"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="48"/>
+      <c r="I61" s="48"/>
+      <c r="J61" s="48"/>
+      <c r="K61" s="48"/>
+      <c r="L61" s="48"/>
+      <c r="M61" s="48"/>
+      <c r="N61" s="48"/>
+      <c r="O61" s="48"/>
+      <c r="P61" s="48"/>
+      <c r="Q61" s="48"/>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A62" s="36" t="s">
+      <c r="A62" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="B62" s="37"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
-      <c r="E62" s="38"/>
-      <c r="F62" s="38"/>
-      <c r="G62" s="38"/>
-      <c r="H62" s="38"/>
-      <c r="I62" s="38"/>
-      <c r="J62" s="38"/>
-      <c r="K62" s="38"/>
-      <c r="L62" s="38"/>
-      <c r="M62" s="38"/>
-      <c r="N62" s="38"/>
-      <c r="O62" s="38"/>
-      <c r="P62" s="38"/>
-      <c r="Q62" s="39"/>
+      <c r="B62" s="46"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="46"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="46"/>
+      <c r="H62" s="46"/>
+      <c r="I62" s="46"/>
+      <c r="J62" s="46"/>
+      <c r="K62" s="46"/>
+      <c r="L62" s="46"/>
+      <c r="M62" s="46"/>
+      <c r="N62" s="46"/>
+      <c r="O62" s="46"/>
+      <c r="P62" s="46"/>
+      <c r="Q62" s="46"/>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A63" s="36" t="s">
+      <c r="A63" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="B63" s="37"/>
-      <c r="C63" s="44"/>
-      <c r="D63" s="44"/>
-      <c r="E63" s="44"/>
-      <c r="F63" s="44"/>
-      <c r="G63" s="44"/>
-      <c r="H63" s="44"/>
-      <c r="I63" s="38"/>
-      <c r="J63" s="44"/>
-      <c r="K63" s="44"/>
-      <c r="L63" s="44"/>
-      <c r="M63" s="44"/>
-      <c r="N63" s="44"/>
-      <c r="O63" s="38"/>
-      <c r="P63" s="38"/>
-      <c r="Q63" s="39"/>
+      <c r="B63" s="46"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="50"/>
+      <c r="F63" s="50"/>
+      <c r="G63" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="H63" s="50"/>
+      <c r="I63" s="46"/>
+      <c r="J63" s="50"/>
+      <c r="K63" s="50"/>
+      <c r="L63" s="50"/>
+      <c r="M63" s="50"/>
+      <c r="N63" s="50"/>
+      <c r="O63" s="46"/>
+      <c r="P63" s="46"/>
+      <c r="Q63" s="46"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A64" s="36" t="s">
+      <c r="A64" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="B64" s="37"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
-      <c r="E64" s="38"/>
-      <c r="F64" s="38"/>
-      <c r="G64" s="38"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="38"/>
-      <c r="J64" s="38"/>
-      <c r="K64" s="38"/>
-      <c r="L64" s="38"/>
-      <c r="M64" s="38"/>
-      <c r="N64" s="38"/>
-      <c r="O64" s="38"/>
-      <c r="P64" s="38"/>
-      <c r="Q64" s="39"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="36"/>
+      <c r="F64" s="36"/>
+      <c r="G64" s="36"/>
+      <c r="H64" s="36"/>
+      <c r="I64" s="36"/>
+      <c r="J64" s="36"/>
+      <c r="K64" s="36"/>
+      <c r="L64" s="36"/>
+      <c r="M64" s="36"/>
+      <c r="N64" s="36"/>
+      <c r="O64" s="36"/>
+      <c r="P64" s="36"/>
+      <c r="Q64" s="37"/>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A65" s="36" t="s">
+      <c r="A65" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="B65" s="37"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="38"/>
-      <c r="E65" s="38"/>
-      <c r="F65" s="38"/>
-      <c r="G65" s="38"/>
-      <c r="H65" s="38"/>
-      <c r="I65" s="38"/>
-      <c r="J65" s="38"/>
-      <c r="K65" s="38"/>
-      <c r="L65" s="38"/>
-      <c r="M65" s="38"/>
-      <c r="N65" s="38"/>
-      <c r="O65" s="38"/>
-      <c r="P65" s="38"/>
-      <c r="Q65" s="39"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="36"/>
+      <c r="E65" s="36"/>
+      <c r="F65" s="36"/>
+      <c r="G65" s="36"/>
+      <c r="H65" s="36"/>
+      <c r="I65" s="36"/>
+      <c r="J65" s="36"/>
+      <c r="K65" s="36"/>
+      <c r="L65" s="36"/>
+      <c r="M65" s="36"/>
+      <c r="N65" s="36"/>
+      <c r="O65" s="36"/>
+      <c r="P65" s="36"/>
+      <c r="Q65" s="37"/>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A66" s="36" t="s">
+      <c r="A66" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="B66" s="37"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="38"/>
-      <c r="G66" s="38"/>
-      <c r="H66" s="38"/>
-      <c r="I66" s="38"/>
-      <c r="J66" s="38"/>
-      <c r="K66" s="38"/>
-      <c r="L66" s="38"/>
-      <c r="M66" s="38"/>
-      <c r="N66" s="38"/>
-      <c r="O66" s="38"/>
-      <c r="P66" s="38"/>
-      <c r="Q66" s="39"/>
+      <c r="B66" s="35"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="36"/>
+      <c r="F66" s="36"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="36"/>
+      <c r="I66" s="36"/>
+      <c r="J66" s="36"/>
+      <c r="K66" s="36"/>
+      <c r="L66" s="36"/>
+      <c r="M66" s="36"/>
+      <c r="N66" s="36"/>
+      <c r="O66" s="36"/>
+      <c r="P66" s="36"/>
+      <c r="Q66" s="37"/>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A67" s="36" t="s">
+      <c r="A67" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="B67" s="37"/>
-      <c r="C67" s="38"/>
-      <c r="D67" s="38"/>
-      <c r="E67" s="38"/>
-      <c r="F67" s="38"/>
-      <c r="G67" s="38"/>
-      <c r="H67" s="38"/>
-      <c r="I67" s="38"/>
-      <c r="J67" s="38"/>
-      <c r="K67" s="38"/>
-      <c r="L67" s="38"/>
-      <c r="M67" s="38"/>
-      <c r="N67" s="38"/>
-      <c r="O67" s="38"/>
-      <c r="P67" s="38"/>
-      <c r="Q67" s="39"/>
+      <c r="B67" s="35"/>
+      <c r="C67" s="36"/>
+      <c r="D67" s="36"/>
+      <c r="E67" s="36"/>
+      <c r="F67" s="36"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="36"/>
+      <c r="I67" s="36"/>
+      <c r="J67" s="36"/>
+      <c r="K67" s="36"/>
+      <c r="L67" s="36"/>
+      <c r="M67" s="36"/>
+      <c r="N67" s="36"/>
+      <c r="O67" s="36"/>
+      <c r="P67" s="36"/>
+      <c r="Q67" s="37"/>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A68" s="36" t="s">
+      <c r="A68" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="37"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="38"/>
-      <c r="E68" s="38"/>
-      <c r="F68" s="38"/>
-      <c r="G68" s="38"/>
-      <c r="H68" s="38"/>
-      <c r="I68" s="38"/>
-      <c r="J68" s="38"/>
-      <c r="K68" s="38"/>
-      <c r="L68" s="38"/>
-      <c r="M68" s="38"/>
-      <c r="N68" s="38"/>
-      <c r="O68" s="38"/>
-      <c r="P68" s="38"/>
-      <c r="Q68" s="39"/>
+      <c r="B68" s="35"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="36"/>
+      <c r="E68" s="36"/>
+      <c r="F68" s="36"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="36"/>
+      <c r="I68" s="36"/>
+      <c r="J68" s="36"/>
+      <c r="K68" s="36"/>
+      <c r="L68" s="36"/>
+      <c r="M68" s="36"/>
+      <c r="N68" s="36"/>
+      <c r="O68" s="36"/>
+      <c r="P68" s="36"/>
+      <c r="Q68" s="37"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A69" s="36" t="s">
+      <c r="A69" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="B69" s="37"/>
-      <c r="C69" s="38"/>
-      <c r="D69" s="38"/>
-      <c r="E69" s="38"/>
-      <c r="F69" s="38"/>
-      <c r="G69" s="38"/>
-      <c r="H69" s="38"/>
-      <c r="I69" s="38"/>
-      <c r="J69" s="38"/>
-      <c r="K69" s="38"/>
-      <c r="L69" s="38"/>
-      <c r="M69" s="38"/>
-      <c r="N69" s="38"/>
-      <c r="O69" s="38"/>
-      <c r="P69" s="38"/>
-      <c r="Q69" s="39"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="36"/>
+      <c r="F69" s="36"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="36"/>
+      <c r="I69" s="36"/>
+      <c r="J69" s="36"/>
+      <c r="K69" s="36"/>
+      <c r="L69" s="36"/>
+      <c r="M69" s="36"/>
+      <c r="N69" s="36"/>
+      <c r="O69" s="36"/>
+      <c r="P69" s="36"/>
+      <c r="Q69" s="37"/>
     </row>
     <row r="70" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="43" t="s">
+      <c r="A70" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="B70" s="52"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="53"/>
-      <c r="G70" s="53"/>
-      <c r="H70" s="53"/>
-      <c r="I70" s="53"/>
-      <c r="J70" s="53"/>
-      <c r="K70" s="53"/>
-      <c r="L70" s="53"/>
-      <c r="M70" s="53"/>
-      <c r="N70" s="53"/>
-      <c r="O70" s="53"/>
-      <c r="P70" s="53"/>
-      <c r="Q70" s="54"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="43"/>
+      <c r="D70" s="43"/>
+      <c r="E70" s="43"/>
+      <c r="F70" s="43"/>
+      <c r="G70" s="43"/>
+      <c r="H70" s="43"/>
+      <c r="I70" s="43"/>
+      <c r="J70" s="43"/>
+      <c r="K70" s="43"/>
+      <c r="L70" s="43"/>
+      <c r="M70" s="43"/>
+      <c r="N70" s="43"/>
+      <c r="O70" s="43"/>
+      <c r="P70" s="43"/>
+      <c r="Q70" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>